<commit_message>
Added percentage of population affected
</commit_message>
<xml_diff>
--- a/covid19_homeless_impact.xlsx
+++ b/covid19_homeless_impact.xlsx
@@ -1,31 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mina\Desktop\BST\DSO110-Final Group Project\DFT-Repo\DFT_Final_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elijah Farmer\Documents\Final project\DFT_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBE5645-8A32-4B72-A5EE-775FDFEBF34D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDAECE4-2B92-47AD-AE6D-D6F82388ACA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30600" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F654852-F8EC-43C0-8FD9-CAEF4A4B67A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F654852-F8EC-43C0-8FD9-CAEF4A4B67A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>date</t>
   </si>
@@ -49,6 +57,12 @@
   </si>
   <si>
     <t>cumulative_homeless_cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_population_by_percentage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_homless_population_by_percentage </t>
   </si>
 </sst>
 </file>
@@ -465,23 +479,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A87887-1679-4790-BEDE-AA8FC91746CC}">
-  <dimension ref="A1:H91"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="3" customWidth="1"/>
     <col min="2" max="3" width="17" style="3" customWidth="1"/>
     <col min="4" max="5" width="17" style="7" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="10" customWidth="1"/>
     <col min="8" max="8" width="27" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.21875" customWidth="1"/>
+    <col min="10" max="10" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,8 +522,14 @@
       <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>43936</v>
       </c>
@@ -532,8 +554,16 @@
       <c r="H2" s="10">
         <v>119</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>(H2/151278)*100</f>
+        <v>7.8663123520934963E-2</v>
+      </c>
+      <c r="J2">
+        <f>(G2/39510000)*100</f>
+        <v>6.4259681093394083E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>43937</v>
       </c>
@@ -558,8 +588,16 @@
       <c r="H3" s="10">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f t="shared" ref="I3:I66" si="0">(H3/151278)*100</f>
+        <v>7.9324158172371401E-2</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J66" si="1">(G3/39510000)*100</f>
+        <v>6.7542394330549232E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>43938</v>
       </c>
@@ -584,8 +622,16 @@
       <c r="H4" s="10">
         <v>123</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>8.1307262126680685E-2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>7.0050620096178184E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>43939</v>
       </c>
@@ -610,8 +656,16 @@
       <c r="H5" s="10">
         <v>123</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>8.1307262126680685E-2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>7.3796507213363713E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>43940</v>
       </c>
@@ -636,8 +690,16 @@
       <c r="H6" s="10">
         <v>126</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>8.3290366080989955E-2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>7.7223487724626672E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43941</v>
       </c>
@@ -662,8 +724,16 @@
       <c r="H7" s="10">
         <v>127</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>8.3951400732426393E-2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>7.9552012148823084E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>43942</v>
       </c>
@@ -688,8 +758,16 @@
       <c r="H8" s="10">
         <v>128</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>8.4612435383862816E-2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>8.5259427992913195E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>43943</v>
       </c>
@@ -714,8 +792,16 @@
       <c r="H9" s="10">
         <v>129</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>8.527347003529924E-2</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>8.9800050620096189E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>43944</v>
       </c>
@@ -740,8 +826,16 @@
       <c r="H10" s="10">
         <v>129</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>8.527347003529924E-2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>9.4538091622374087E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>43945</v>
       </c>
@@ -766,8 +860,16 @@
       <c r="H11" s="10">
         <v>131</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>8.6595539338172101E-2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>0.10012908124525435</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>43946</v>
       </c>
@@ -792,8 +894,16 @@
       <c r="H12" s="10">
         <v>131</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>8.6595539338172101E-2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>0.10466970387243736</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>43947</v>
       </c>
@@ -818,8 +928,16 @@
       <c r="H13" s="10">
         <v>133</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>8.7917608641044961E-2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>0.10723361174386231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>43948</v>
       </c>
@@ -844,8 +962,16 @@
       <c r="H14" s="10">
         <v>136</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>8.9900712595354246E-2</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>0.1102480384712731</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>43949</v>
       </c>
@@ -870,8 +996,16 @@
       <c r="H15" s="10">
         <v>138</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>9.1222781898227107E-2</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>0.1138243482662617</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>43950</v>
       </c>
@@ -896,8 +1030,16 @@
       <c r="H16" s="10">
         <v>141</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>9.3205885852536391E-2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>0.11684130599848139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>43951</v>
       </c>
@@ -922,8 +1064,16 @@
       <c r="H17" s="10">
         <v>142</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>9.3866920503972814E-2</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>0.12337889141989371</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>43952</v>
       </c>
@@ -948,8 +1098,16 @@
       <c r="H18" s="10">
         <v>143</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>9.4527955155409252E-2</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>0.12687927107061503</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>43953</v>
       </c>
@@ -974,8 +1132,16 @@
       <c r="H19" s="10">
         <v>147</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>9.717209376115496E-2</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>0.13167805618830677</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>43954</v>
       </c>
@@ -1000,8 +1166,16 @@
       <c r="H20" s="10">
         <v>147</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>9.717209376115496E-2</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>0.13502151354087571</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>43955</v>
       </c>
@@ -1026,8 +1200,16 @@
       <c r="H21" s="10">
         <v>149</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>9.8494163064027807E-2</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>0.13895975702353836</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>43956</v>
       </c>
@@ -1052,8 +1234,16 @@
       <c r="H22" s="10">
         <v>150</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>9.9155197715464244E-2</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>0.14144267274107822</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>43957</v>
       </c>
@@ -1078,8 +1268,16 @@
       <c r="H23" s="10">
         <v>154</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>0.10179933632120995</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>0.1479524171095925</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>43958</v>
       </c>
@@ -1104,8 +1302,16 @@
       <c r="H24" s="10">
         <v>154</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>0.10179933632120995</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>0.15341938749683623</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>43959</v>
       </c>
@@ -1130,8 +1336,16 @@
       <c r="H25" s="10">
         <v>154</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>0.10179933632120995</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>0.15729688686408502</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>43960</v>
       </c>
@@ -1156,8 +1370,16 @@
       <c r="H26" s="10">
         <v>154</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>0.10179933632120995</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>0.16147810680840294</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>43961</v>
       </c>
@@ -1182,8 +1404,16 @@
       <c r="H27" s="10">
         <v>154</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>0.10179933632120995</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>0.16849405213869906</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>43962</v>
       </c>
@@ -1208,8 +1438,16 @@
       <c r="H28" s="10">
         <v>155</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>0.10246037097264638</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>0.17109592508225765</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>43963</v>
       </c>
@@ -1234,8 +1472,16 @@
       <c r="H29" s="10">
         <v>155</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>0.10246037097264638</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>0.17547203239686157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>43964</v>
       </c>
@@ -1260,8 +1506,16 @@
       <c r="H30" s="10">
         <v>155</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>0.10246037097264638</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>0.17965072133637053</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>43965</v>
       </c>
@@ -1286,8 +1540,16 @@
       <c r="H31" s="10">
         <v>155</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>0.10246037097264638</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>0.18425208807896734</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>43966</v>
       </c>
@@ -1312,8 +1574,16 @@
       <c r="H32" s="10">
         <v>155</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>0.10246037097264638</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>0.189498861047836</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>43967</v>
       </c>
@@ -1338,8 +1608,16 @@
       <c r="H33" s="10">
         <v>155</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>0.10246037097264638</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>0.19411035180966846</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>43968</v>
       </c>
@@ -1364,8 +1642,16 @@
       <c r="H34" s="10">
         <v>156</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>0.10312140562408281</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>0.19925335358137181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>43969</v>
       </c>
@@ -1390,8 +1676,16 @@
       <c r="H35" s="10">
         <v>157</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>0.10378244027551924</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="1"/>
+        <v>0.20290053151100987</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>43970</v>
       </c>
@@ -1416,8 +1710,16 @@
       <c r="H36" s="10">
         <v>158</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>0.10444347492695567</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>0.20632245001265503</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>43971</v>
       </c>
@@ -1442,8 +1744,16 @@
       <c r="H37" s="10">
         <v>159</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>0.1051045095783921</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="1"/>
+        <v>0.21200708681346497</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>43972</v>
       </c>
@@ -1468,8 +1778,16 @@
       <c r="H38" s="10">
         <v>159</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>0.1051045095783921</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>0.21771197165274614</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>43973</v>
       </c>
@@ -1494,8 +1812,16 @@
       <c r="H39" s="10">
         <v>159</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>0.1051045095783921</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>0.22287015945330296</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>43974</v>
       </c>
@@ -1520,8 +1846,16 @@
       <c r="H40" s="10">
         <v>159</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>0.1051045095783921</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="1"/>
+        <v>0.22850164515312582</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>43975</v>
       </c>
@@ -1546,8 +1880,16 @@
       <c r="H41" s="10">
         <v>160</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <f t="shared" si="0"/>
+        <v>0.10576554422982852</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="1"/>
+        <v>0.23427992913186538</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>43976</v>
       </c>
@@ -1572,8 +1914,16 @@
       <c r="H42" s="10">
         <v>160</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>0.10576554422982852</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="1"/>
+        <v>0.23808909136927361</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>43977</v>
       </c>
@@ -1598,8 +1948,16 @@
       <c r="H43" s="10">
         <v>160</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>0.10576554422982852</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="1"/>
+        <v>0.24416603391546446</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43978</v>
       </c>
@@ -1624,8 +1982,16 @@
       <c r="H44" s="10">
         <v>161</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>0.10642657888126496</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="1"/>
+        <v>0.25181473044798786</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>43979</v>
       </c>
@@ -1650,8 +2016,16 @@
       <c r="H45" s="10">
         <v>161</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <f t="shared" si="0"/>
+        <v>0.10642657888126496</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="1"/>
+        <v>0.25581118704125538</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>43980</v>
       </c>
@@ -1676,8 +2050,16 @@
       <c r="H46" s="10">
         <v>163</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <f t="shared" si="0"/>
+        <v>0.1077486481841378</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="1"/>
+        <v>0.26275120222728421</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>43983</v>
       </c>
@@ -1702,8 +2084,16 @@
       <c r="H47" s="10">
         <v>167</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <f t="shared" si="0"/>
+        <v>0.11039278678988353</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="1"/>
+        <v>0.2833485193621868</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>43984</v>
       </c>
@@ -1728,8 +2118,16 @@
       <c r="H48" s="10">
         <v>167</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <f t="shared" si="0"/>
+        <v>0.11039278678988353</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="1"/>
+        <v>0.29038977474057204</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>43985</v>
       </c>
@@ -1754,8 +2152,16 @@
       <c r="H49" s="10">
         <v>168</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <f t="shared" si="0"/>
+        <v>0.11105382144131995</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="1"/>
+        <v>0.2966717286762845</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>43986</v>
       </c>
@@ -1780,8 +2186,16 @@
       <c r="H50" s="10">
         <v>170</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <f t="shared" si="0"/>
+        <v>0.11237589074419281</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="1"/>
+        <v>0.30213616805871929</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>43987</v>
       </c>
@@ -1806,8 +2220,16 @@
       <c r="H51" s="10">
         <v>171</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <f t="shared" si="0"/>
+        <v>0.11303692539562923</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="1"/>
+        <v>0.30927360161984307</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>43990</v>
       </c>
@@ -1832,8 +2254,16 @@
       <c r="H52" s="10">
         <v>173</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <f t="shared" si="0"/>
+        <v>0.11435899469850209</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="1"/>
+        <v>0.33069349531764114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>43991</v>
       </c>
@@ -1858,8 +2288,16 @@
       <c r="H53" s="10">
         <v>174</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <f t="shared" si="0"/>
+        <v>0.11502002934993853</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="1"/>
+        <v>0.3386889395089851</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>43992</v>
       </c>
@@ -1884,8 +2322,16 @@
       <c r="H54" s="10">
         <v>174</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <f t="shared" si="0"/>
+        <v>0.11502002934993853</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="1"/>
+        <v>0.3459402682865097</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>43993</v>
       </c>
@@ -1910,8 +2356,16 @@
       <c r="H55" s="10">
         <v>175</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <f t="shared" si="0"/>
+        <v>0.11568106400137496</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="1"/>
+        <v>0.35361933687674008</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>43994</v>
       </c>
@@ -1936,8 +2390,16 @@
       <c r="H56" s="10">
         <v>175</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <f t="shared" si="0"/>
+        <v>0.11568106400137496</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="1"/>
+        <v>0.36304479878511769</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>43997</v>
       </c>
@@ -1962,8 +2424,16 @@
       <c r="H57" s="10">
         <v>176</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <f t="shared" si="0"/>
+        <v>0.11634209865281138</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="1"/>
+        <v>0.3855960516324981</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>43998</v>
       </c>
@@ -1988,8 +2458,16 @@
       <c r="H58" s="10">
         <v>176</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <f t="shared" si="0"/>
+        <v>0.11634209865281138</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="1"/>
+        <v>0.39414325487218421</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>43999</v>
       </c>
@@ -2014,8 +2492,16 @@
       <c r="H59" s="10">
         <v>177</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59">
+        <f t="shared" si="0"/>
+        <v>0.11700313330424782</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="1"/>
+        <v>0.40233105542900538</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>44000</v>
       </c>
@@ -2040,8 +2526,16 @@
       <c r="H60" s="10">
         <v>178</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <f t="shared" si="0"/>
+        <v>0.11766416795568424</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="1"/>
+        <v>0.41204252088078969</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>44001</v>
       </c>
@@ -2066,8 +2560,16 @@
       <c r="H61" s="10">
         <v>181</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <f t="shared" si="0"/>
+        <v>0.11964727190999352</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="1"/>
+        <v>0.4230144267274108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>44004</v>
       </c>
@@ -2092,8 +2594,16 @@
       <c r="H62" s="10">
         <v>187</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <f t="shared" si="0"/>
+        <v>0.12361347981861209</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="1"/>
+        <v>0.45218172614527968</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>44005</v>
       </c>
@@ -2118,8 +2628,16 @@
       <c r="H63" s="10">
         <v>191</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63">
+        <f t="shared" si="0"/>
+        <v>0.12625761842435781</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="1"/>
+        <v>0.46764110351809668</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>44006</v>
       </c>
@@ -2144,8 +2662,16 @@
       <c r="H64" s="10">
         <v>191</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64">
+        <f t="shared" si="0"/>
+        <v>0.12625761842435781</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="1"/>
+        <v>0.48462920779549484</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>44007</v>
       </c>
@@ -2170,8 +2696,16 @@
       <c r="H65" s="10">
         <v>192</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65">
+        <f t="shared" si="0"/>
+        <v>0.12691865307579425</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="1"/>
+        <v>0.49613768666160463</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>44008</v>
       </c>
@@ -2196,8 +2730,16 @@
       <c r="H66" s="10">
         <v>192</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <f t="shared" si="0"/>
+        <v>0.12691865307579425</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="1"/>
+        <v>0.50901543912933434</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>44011</v>
       </c>
@@ -2222,8 +2764,16 @@
       <c r="H67" s="10">
         <v>197</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <f t="shared" ref="I67:I91" si="2">(H67/151278)*100</f>
+        <v>0.13022382633297636</v>
+      </c>
+      <c r="J67">
+        <f t="shared" ref="J67:J91" si="3">(G67/39510000)*100</f>
+        <v>0.54539863325740323</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>44012</v>
       </c>
@@ -2248,8 +2798,16 @@
       <c r="H68" s="10">
         <v>198</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <f t="shared" si="2"/>
+        <v>0.13088486098441279</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="3"/>
+        <v>0.56604910149329279</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>44013</v>
       </c>
@@ -2274,8 +2832,16 @@
       <c r="H69" s="10">
         <v>199</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <f t="shared" si="2"/>
+        <v>0.13154589563584923</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="3"/>
+        <v>0.5857200708681346</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>44014</v>
       </c>
@@ -2300,8 +2866,16 @@
       <c r="H70" s="10">
         <v>200</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70">
+        <f t="shared" si="2"/>
+        <v>0.13220693028728564</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="3"/>
+        <v>0.60410275879524167</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>44015</v>
       </c>
@@ -2326,8 +2900,16 @@
       <c r="H71" s="10">
         <v>200</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71">
+        <f t="shared" si="2"/>
+        <v>0.13220693028728564</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="3"/>
+        <v>0.62401923563654771</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>44018</v>
       </c>
@@ -2352,8 +2934,16 @@
       <c r="H72" s="10">
         <v>205</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72">
+        <f t="shared" si="2"/>
+        <v>0.1355121035444678</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="3"/>
+        <v>0.6699088838268793</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>44019</v>
       </c>
@@ -2378,8 +2968,16 @@
       <c r="H73" s="10">
         <v>206</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73">
+        <f t="shared" si="2"/>
+        <v>0.13617313819590421</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="3"/>
+        <v>0.68599088838268796</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>44020</v>
       </c>
@@ -2404,8 +3002,16 @@
       <c r="H74" s="10">
         <v>208</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74">
+        <f t="shared" si="2"/>
+        <v>0.13749520749877708</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="3"/>
+        <v>0.71883573778790177</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>44021</v>
       </c>
@@ -2430,8 +3036,16 @@
       <c r="H75" s="10">
         <v>211</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75">
+        <f t="shared" si="2"/>
+        <v>0.13947831145308637</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="3"/>
+        <v>0.74047076689445712</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>44022</v>
       </c>
@@ -2456,8 +3070,16 @@
       <c r="H76" s="10">
         <v>211</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76">
+        <f t="shared" si="2"/>
+        <v>0.13947831145308637</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="3"/>
+        <v>0.76558845861807145</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>44025</v>
       </c>
@@ -2482,8 +3104,16 @@
       <c r="H77" s="10">
         <v>215</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77">
+        <f t="shared" si="2"/>
+        <v>0.14212245005883209</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="3"/>
+        <v>0.821419893697798</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>44026</v>
       </c>
@@ -2508,8 +3138,16 @@
       <c r="H78" s="10">
         <v>219</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78">
+        <f t="shared" si="2"/>
+        <v>0.14476658866457778</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="3"/>
+        <v>0.84372817008352319</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>44027</v>
       </c>
@@ -2534,8 +3172,16 @@
       <c r="H79" s="10">
         <v>221</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79">
+        <f t="shared" si="2"/>
+        <v>0.14608865796745066</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="3"/>
+        <v>0.87626170589724128</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>44028</v>
       </c>
@@ -2560,8 +3206,16 @@
       <c r="H80" s="10">
         <v>223</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80">
+        <f t="shared" si="2"/>
+        <v>0.1474107272703235</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="3"/>
+        <v>0.89821564160971912</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>44029</v>
       </c>
@@ -2586,8 +3240,16 @@
       <c r="H81" s="10">
         <v>226</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81">
+        <f t="shared" si="2"/>
+        <v>0.14939383122463279</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="3"/>
+        <v>0.92307263983801568</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>44032</v>
       </c>
@@ -2612,8 +3274,16 @@
       <c r="H82" s="10">
         <v>233</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82">
+        <f t="shared" si="2"/>
+        <v>0.1540210737846878</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="3"/>
+        <v>0.97926094659579843</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>44033</v>
       </c>
@@ -2638,8 +3308,16 @@
       <c r="H83" s="10">
         <v>235</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83">
+        <f t="shared" si="2"/>
+        <v>0.15534314308756064</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="3"/>
+        <v>1.0070108833206783</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>44034</v>
       </c>
@@ -2664,8 +3342,16 @@
       <c r="H84" s="10">
         <v>238</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84">
+        <f t="shared" si="2"/>
+        <v>0.15732624704186993</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="3"/>
+        <v>1.0359529233105542</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>44035</v>
       </c>
@@ -2690,8 +3376,16 @@
       <c r="H85" s="10">
         <v>241</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <f t="shared" si="2"/>
+        <v>0.15930935099617924</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="3"/>
+        <v>1.0662768919260945</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>44036</v>
       </c>
@@ -2716,8 +3410,16 @@
       <c r="H86" s="10">
         <v>241</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86">
+        <f t="shared" si="2"/>
+        <v>0.15930935099617924</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="3"/>
+        <v>1.0902885345482156</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>44039</v>
       </c>
@@ -2742,8 +3444,16 @@
       <c r="H87" s="10">
         <v>244</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87">
+        <f t="shared" si="2"/>
+        <v>0.16129245495048852</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="3"/>
+        <v>1.1447431030118957</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>44040</v>
       </c>
@@ -2768,8 +3478,16 @@
       <c r="H88" s="10">
         <v>246</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88">
+        <f t="shared" si="2"/>
+        <v>0.16261452425336137</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="3"/>
+        <v>1.1595064540622626</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>44041</v>
       </c>
@@ -2794,8 +3512,16 @@
       <c r="H89" s="10">
         <v>246</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89">
+        <f t="shared" si="2"/>
+        <v>0.16261452425336137</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="3"/>
+        <v>1.1915008858516831</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>44042</v>
       </c>
@@ -2820,8 +3546,16 @@
       <c r="H90" s="10">
         <v>246</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90">
+        <f t="shared" si="2"/>
+        <v>0.16261452425336137</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="3"/>
+        <v>1.2273171349025562</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>44043</v>
       </c>
@@ -2845,6 +3579,14 @@
       </c>
       <c r="H91" s="10">
         <v>246</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="2"/>
+        <v>0.16261452425336137</v>
+      </c>
+      <c r="J91">
+        <f>(G91/39510000)*100</f>
+        <v>1.2476183244748165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>